<commit_message>
See https://github.com/open-geodata/sp_cetesb_infoaguas/commit/cb423a6110b9973070cd6044f506707568c0ea73 from refs/heads/main
</commit_message>
<xml_diff>
--- a/assets/sp_cetesb_infoaguas/excel/ALVE02800.xlsx
+++ b/assets/sp_cetesb_infoaguas/excel/ALVE02800.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,18 +506,18 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Nitrogênio Kjeldahl</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>51.50000000</t>
+          <t>7.42000000</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>U.pH</t>
         </is>
       </c>
     </row>
@@ -532,18 +532,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sólido Total</t>
+          <t>Turbidez</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>404.00000000</t>
+          <t>44.00000000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UNT</t>
         </is>
       </c>
     </row>
@@ -558,18 +558,18 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Nitrogênio Amoniacal</t>
+          <t>Temperatura da Água</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>36.90000000</t>
+          <t>27.00000000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>ºC</t>
         </is>
       </c>
     </row>
@@ -584,13 +584,13 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fósforo Total</t>
+          <t>Sólido Total</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4.21000000</t>
+          <t>404.00000000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -610,13 +610,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Oxigênio Dissolvido</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.09000000</t>
+          <t>100.00000000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -636,18 +640,18 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Escherichia coli</t>
+          <t>Oxigênio Dissolvido</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6900000.00000000</t>
+          <t>0.09000000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>UFC/100mL</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -662,18 +666,18 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>Nitrogênio Amoniacal</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7.42000000</t>
+          <t>36.90000000</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>U.pH</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -688,13 +692,13 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DQO (relativo a carbono)</t>
+          <t>Fósforo Total</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>161.00000000</t>
+          <t>4.21000000</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -714,18 +718,18 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Temperatura da Água</t>
+          <t>Escherichia coli</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>27.00000000</t>
+          <t>6900000.00000000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ºC</t>
+          <t>UFC/100mL</t>
         </is>
       </c>
     </row>
@@ -740,13 +744,13 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>DBO (5, 20)</t>
+          <t>DQO (relativo a carbono)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>116.00000000</t>
+          <t>161.00000000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -766,18 +770,18 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Turbidez</t>
+          <t>DBO (5, 20)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>44.00000000</t>
+          <t>116.00000000</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>UNT</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -792,17 +796,13 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sólido Suspenso Total</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>&lt;</t>
-        </is>
-      </c>
+          <t>Nitrogênio Kjeldahl</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>100.00000000</t>
+          <t>51.50000000</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -848,18 +848,18 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Temperatura da Água</t>
+          <t>Fósforo Total</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>21.70000000</t>
+          <t>5.00000000</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ºC</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -874,18 +874,18 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Oxigênio Dissolvido</t>
+          <t>Turbidez</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.18000000</t>
+          <t>93.56000000</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UNT</t>
         </is>
       </c>
     </row>
@@ -900,18 +900,18 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Turbidez</t>
+          <t>Temperatura da Água</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>93.56000000</t>
+          <t>21.70000000</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>UNT</t>
+          <t>ºC</t>
         </is>
       </c>
     </row>
@@ -952,18 +952,18 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Condutividade</t>
+          <t>Nitrogênio Amoniacal</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>715.00000000</t>
+          <t>39.10000000</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>µS/cm</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -978,13 +978,13 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Nitrogênio Kjeldahl</t>
+          <t>Sólido Total</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>47.90000000</t>
+          <t>538.00000000</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1004,13 +1004,13 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Sólido Suspenso Total</t>
+          <t>Carbono Orgânico Total</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>158.00000000</t>
+          <t>94.20000000</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1030,18 +1030,18 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>DQO (relativo a carbono)</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>290.00000000</t>
+          <t>7.37000000</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>U.pH</t>
         </is>
       </c>
     </row>
@@ -1056,18 +1056,18 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>Nitrogênio Kjeldahl</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>7.37000000</t>
+          <t>47.90000000</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>U.pH</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1082,13 +1082,13 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Sólido Total</t>
+          <t>DQO (relativo a carbono)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>538.00000000</t>
+          <t>290.00000000</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1108,13 +1108,13 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Carbono Orgânico Total</t>
+          <t>Sólido Suspenso Total</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>94.20000000</t>
+          <t>158.00000000</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1160,18 +1160,18 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Nitrogênio Amoniacal</t>
+          <t>Condutividade</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>39.10000000</t>
+          <t>715.00000000</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>µS/cm</t>
         </is>
       </c>
     </row>
@@ -1186,13 +1186,13 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Fósforo Total</t>
+          <t>Oxigênio Dissolvido</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5.00000000</t>
+          <t>0.18000000</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1212,13 +1212,13 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Fósforo Total</t>
+          <t>Carbono Orgânico Total</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4.00000000</t>
+          <t>73.00000000</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1238,13 +1238,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Nitrogênio Amoniacal</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>28.20000000</t>
+          <t>100.00000000</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1264,18 +1268,18 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Carbono Orgânico Total</t>
+          <t>Temperatura da Água</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>73.00000000</t>
+          <t>20.00000000</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>ºC</t>
         </is>
       </c>
     </row>
@@ -1290,18 +1294,18 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Sólido Total</t>
+          <t>Escherichia coli</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>340.00000000</t>
+          <t>5800000.00000000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UFC/100mL</t>
         </is>
       </c>
     </row>
@@ -1316,22 +1320,18 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Sólido Suspenso Total</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>&lt;</t>
-        </is>
-      </c>
+          <t>Turbidez</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>100.00000000</t>
+          <t>50.09000000</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UNT</t>
         </is>
       </c>
     </row>
@@ -1346,18 +1346,18 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>Oxigênio Dissolvido</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>7.52000000</t>
+          <t>1.44000000</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>U.pH</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1372,18 +1372,18 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Escherichia coli</t>
+          <t>Nitrogênio Kjeldahl</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>5800000.00000000</t>
+          <t>41.40000000</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>UFC/100mL</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1398,13 +1398,13 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Oxigênio Dissolvido</t>
+          <t>Sólido Total</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.44000000</t>
+          <t>340.00000000</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1450,18 +1450,18 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Condutividade</t>
+          <t>Fósforo Total</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>595.00000000</t>
+          <t>4.00000000</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>µS/cm</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1476,18 +1476,18 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Turbidez</t>
+          <t>Condutividade</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>50.09000000</t>
+          <t>595.00000000</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>UNT</t>
+          <t>µS/cm</t>
         </is>
       </c>
     </row>
@@ -1502,18 +1502,18 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>DBO (5, 20)</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>66.80000000</t>
+          <t>7.52000000</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>U.pH</t>
         </is>
       </c>
     </row>
@@ -1528,18 +1528,18 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Temperatura da Água</t>
+          <t>DBO (5, 20)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>20.00000000</t>
+          <t>66.80000000</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>ºC</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1554,13 +1554,13 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Nitrogênio Kjeldahl</t>
+          <t>Nitrogênio Amoniacal</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
-          <t>41.40000000</t>
+          <t>28.20000000</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1580,18 +1580,18 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Turbidez</t>
+          <t>Nitrogênio Amoniacal</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
-          <t>37.70000000</t>
+          <t>12.60000000</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>UNT</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1632,13 +1632,13 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Oxigênio Dissolvido</t>
+          <t>Carbono Orgânico Total</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.97000000</t>
+          <t>44.70000000</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1658,17 +1658,13 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Sólido Suspenso Total</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>&lt;</t>
-        </is>
-      </c>
+          <t>Oxigênio Dissolvido</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>100.00000000</t>
+          <t>1.97000000</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1688,18 +1684,22 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Temperatura da Água</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr"/>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>24.30000000</t>
+          <t>100.00000000</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>ºC</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1714,18 +1714,18 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Fósforo Total</t>
+          <t>Temperatura da Água</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>3.17000000</t>
+          <t>24.30000000</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>ºC</t>
         </is>
       </c>
     </row>
@@ -1740,13 +1740,13 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sólido Total</t>
+          <t>Fósforo Total</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>318.00000000</t>
+          <t>3.17000000</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1766,18 +1766,18 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Escherichia coli</t>
+          <t>Sólido Total</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>6600000.00000000</t>
+          <t>318.00000000</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>UFC/100mL</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1792,18 +1792,18 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>DQO (relativo a carbono)</t>
+          <t>Condutividade</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>148.00000000</t>
+          <t>542.00000000</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>µS/cm</t>
         </is>
       </c>
     </row>
@@ -1818,18 +1818,18 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>DBO (5, 20)</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>90.60000000</t>
+          <t>7.56000000</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>U.pH</t>
         </is>
       </c>
     </row>
@@ -1844,18 +1844,18 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Condutividade</t>
+          <t>DBO (5, 20)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>542.00000000</t>
+          <t>90.60000000</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>µS/cm</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1870,18 +1870,18 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>DQO (relativo a carbono)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>7.56000000</t>
+          <t>148.00000000</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>U.pH</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -1896,18 +1896,18 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Carbono Orgânico Total</t>
+          <t>Escherichia coli</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>44.70000000</t>
+          <t>6600000.00000000</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UFC/100mL</t>
         </is>
       </c>
     </row>
@@ -1922,18 +1922,18 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Nitrogênio Amoniacal</t>
+          <t>Turbidez</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>12.60000000</t>
+          <t>37.70000000</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UNT</t>
         </is>
       </c>
     </row>
@@ -1948,17 +1948,13 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Sólido Suspenso Total</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>&lt;</t>
-        </is>
-      </c>
+          <t>DBO (5, 20)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>100.00000000</t>
+          <t>71.30000000</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -1978,13 +1974,13 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Sólido Total</t>
+          <t>Carbono Orgânico Total</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>292.00000000</t>
+          <t>50.50000000</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2004,18 +2000,18 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Turbidez</t>
+          <t>Temperatura da Água</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>36.47000000</t>
+          <t>26.00000000</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>UNT</t>
+          <t>ºC</t>
         </is>
       </c>
     </row>
@@ -2030,13 +2026,13 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Nitrogênio Kjeldahl</t>
+          <t>DQO (relativo a carbono)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>36.10000000</t>
+          <t>103.00000000</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2056,18 +2052,18 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>Sólido Total</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
         <is>
-          <t>7.60000000</t>
+          <t>292.00000000</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>U.pH</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -2082,13 +2078,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Nitrogênio Amoniacal</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>24.60000000</t>
+          <t>100.00000000</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2108,13 +2108,13 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Fósforo Total</t>
+          <t>Nitrogênio Amoniacal</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
-          <t>2.80000000</t>
+          <t>24.60000000</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2134,18 +2134,18 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Escherichia coli</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
-          <t>11000000.00000000</t>
+          <t>7.60000000</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>UFC/100mL</t>
+          <t>U.pH</t>
         </is>
       </c>
     </row>
@@ -2160,18 +2160,18 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>DQO (relativo a carbono)</t>
+          <t>Turbidez</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
-          <t>103.00000000</t>
+          <t>36.47000000</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UNT</t>
         </is>
       </c>
     </row>
@@ -2186,13 +2186,13 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>DBO (5, 20)</t>
+          <t>Oxigênio Dissolvido</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>71.30000000</t>
+          <t>1.66000000</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2212,18 +2212,18 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Condutividade</t>
+          <t>Escherichia coli</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>557.00000000</t>
+          <t>11000000.00000000</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>µS/cm</t>
+          <t>UFC/100mL</t>
         </is>
       </c>
     </row>
@@ -2238,13 +2238,13 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Carbono Orgânico Total</t>
+          <t>Fósforo Total</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
-          <t>50.50000000</t>
+          <t>2.80000000</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2264,18 +2264,18 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Oxigênio Dissolvido</t>
+          <t>Condutividade</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.66000000</t>
+          <t>557.00000000</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>µS/cm</t>
         </is>
       </c>
     </row>
@@ -2290,18 +2290,18 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Temperatura da Água</t>
+          <t>Nitrogênio Kjeldahl</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
-          <t>26.00000000</t>
+          <t>36.10000000</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>ºC</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -2316,18 +2316,18 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Turbidez</t>
+          <t>pH</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t>64.66000000</t>
+          <t>7.52000000</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>UNT</t>
+          <t>U.pH</t>
         </is>
       </c>
     </row>
@@ -2342,13 +2342,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Nitrogênio Amoniacal</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>25.10000000</t>
+          <t>100.00000000</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2368,13 +2372,13 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Sólido Total</t>
+          <t>Oxigênio Dissolvido</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
         <is>
-          <t>324.00000000</t>
+          <t>0.82000000</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -2394,22 +2398,18 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Sólido Suspenso Total</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>&lt;</t>
-        </is>
-      </c>
+          <t>Condutividade</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
         <is>
-          <t>100.00000000</t>
+          <t>573.00000000</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>µS/cm</t>
         </is>
       </c>
     </row>
@@ -2424,18 +2424,18 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Oxigênio Dissolvido</t>
+          <t>Temperatura da Água</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
         <is>
-          <t>29.70000000</t>
+          <t>26.30000000</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>ºC</t>
         </is>
       </c>
     </row>
@@ -2450,13 +2450,13 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Nitrogênio Kjeldahl</t>
+          <t>Carbono Orgânico Total</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr">
         <is>
-          <t>29.70000000</t>
+          <t>42.50000000</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -2476,13 +2476,13 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Fósforo Total</t>
+          <t>DBO (5, 20)</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr">
         <is>
-          <t>3.00000000</t>
+          <t>78.40000000</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -2502,18 +2502,18 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Escherichia coli</t>
+          <t>Sólido Total</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
-          <t>7800000.00000000</t>
+          <t>324.00000000</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>UFC/100mL</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -2528,13 +2528,13 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>DQO (relativo a carbono)</t>
+          <t>Nitrogênio Amoniacal</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr">
         <is>
-          <t>115.00000000</t>
+          <t>25.10000000</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -2554,13 +2554,13 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>DBO (5, 20)</t>
+          <t>DQO (relativo a carbono)</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr">
         <is>
-          <t>78.40000000</t>
+          <t>115.00000000</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -2580,18 +2580,18 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Condutividade</t>
+          <t>Turbidez</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
-          <t>573.00000000</t>
+          <t>64.66000000</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>µS/cm</t>
+          <t>UNT</t>
         </is>
       </c>
     </row>
@@ -2606,18 +2606,18 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Carbono Orgânico Total</t>
+          <t>Escherichia coli</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr">
         <is>
-          <t>42.50000000</t>
+          <t>7800000.00000000</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>mg/L</t>
+          <t>UFC/100mL</t>
         </is>
       </c>
     </row>
@@ -2632,18 +2632,18 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Temperatura da Água</t>
+          <t>Fósforo Total</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr">
         <is>
-          <t>26.30000000</t>
+          <t>3.00000000</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>ºC</t>
+          <t>mg/L</t>
         </is>
       </c>
     </row>
@@ -2658,16 +2658,1458 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>pH</t>
+          <t>Nitrogênio Kjeldahl</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr">
         <is>
-          <t>7.52000000</t>
+          <t>29.70000000</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>100.00000000</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>7.59000000</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>U.pH</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Sólido Total</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>232.00000000</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Temperatura da Água</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>20.50000000</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>ºC</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Turbidez</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>27.80000000</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>UNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Nitrogênio Kjeldahl</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>28.10000000</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Fósforo Total</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>2.00000000</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Oxigênio Dissolvido</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>2.84000000</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Carbono Orgânico Total</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>32.60000000</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>DQO (relativo a carbono)</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>80.20000000</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Escherichia coli</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>5300000.00000000</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>UFC/100mL</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Condutividade</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>453.70000000</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>µS/cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Nitrogênio Amoniacal</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>19.30000000</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="n">
+        <v>44308.44444444445</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>DBO (5, 20)</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>64.90000000</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>DBO (5, 20)</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>90.70000000</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Escherichia coli</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>5600000.00000000</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>UFC/100mL</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Turbidez</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>31.70000000</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>UNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B103" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Sólido Total</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>292.00000000</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Carbono Orgânico Total</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>47.20000000</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Temperatura da Água</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>19.00000000</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>ºC</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B106" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Fósforo Total</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>4.50000000</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Nitrogênio Kjeldahl</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>51.60000000</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>DQO (relativo a carbono)</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>153.00000000</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>100.00000000</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>7.57000000</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>U.pH</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B111" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Oxigênio Dissolvido</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>0.30000000</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B112" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Nitrogênio Amoniacal</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>38.70000000</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B113" s="2" t="n">
+        <v>44371.43055555555</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Condutividade</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>635.00000000</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>µS/cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B114" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Temperatura da Água</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>20.30000000</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>ºC</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B115" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Oxigênio Dissolvido</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0.29000000</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>DQO (relativo a carbono)</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>221.00000000</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>DBO (5, 20)</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>172.00000000</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Condutividade</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>744.00000000</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>µS/cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Carbono Orgânico Total</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>90.40000000</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Fósforo Total</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>5.74000000</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Sólido Total</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>404.00000000</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B122" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Nitrogênio Amoniacal</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>43.50000000</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B123" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>7.67000000</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>U.pH</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>104.00000000</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Nitrogênio Kjeldahl</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>56.50000000</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Escherichia coli</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>5900000.00000000</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>UFC/100mL</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B127" s="2" t="n">
+        <v>44425.4375</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Turbidez</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>54.50000000</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>UNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Condutividade</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>621.00000000</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>µS/cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Turbidez</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>29.00000000</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>UNT</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B130" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Escherichia coli</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>14000000.00000000</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>UFC/100mL</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B131" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Carbono Orgânico Total</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr"/>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>48.90000000</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B132" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Temperatura da Água</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>21.30000000</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>ºC</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B133" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Oxigênio Dissolvido</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>0.21000000</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B134" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Fósforo Total</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>4.05000000</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Sólido Total</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>312.00000000</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Nitrogênio Amoniacal</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>31.20000000</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Sólido Suspenso Total</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>100.00000000</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Nitrogênio Kjeldahl</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>44.50000000</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>DBO (5, 20)</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>79.80000000</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>ALVE02800</t>
+        </is>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>44495.43055555555</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>pH</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>7.49000000</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
         <is>
           <t>U.pH</t>
         </is>

</xml_diff>